<commit_message>
Modified files on B3
</commit_message>
<xml_diff>
--- a/seamonitor/backend/register/admin.xlsx
+++ b/seamonitor/backend/register/admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\软件工程\Lab5项目管理\git提交\seamonitor\backend\register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5199A784-7EA4-4DF5-98E9-CDC3F09E61DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC06122-C416-4F20-AF53-49040C05EB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,9 +226,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -571,7 +570,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.55000000000000004"/>
@@ -763,11 +762,11 @@
       <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>49</v>
       </c>
       <c r="C17">
-        <v>123456</v>
+        <v>12345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>